<commit_message>
Update estado del arte
</commit_message>
<xml_diff>
--- a/A00056992/Estado del arte.xlsx
+++ b/A00056992/Estado del arte.xlsx
@@ -47,9 +47,6 @@
     <t>Orientado al proceso asistencial</t>
   </si>
   <si>
-    <t>Es una plicación web</t>
-  </si>
-  <si>
     <t>Es un proceso automatizado</t>
   </si>
   <si>
@@ -71,10 +68,13 @@
     <t>Tecnologias web</t>
   </si>
   <si>
-    <t>Angular,  Laravel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enfocado en la eficiencia y seguridad del control de acceso </t>
+  </si>
+  <si>
+    <t>Es una aplicación web</t>
+  </si>
+  <si>
+    <t>Tecnologías web</t>
   </si>
 </sst>
 </file>
@@ -163,28 +163,28 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -470,7 +470,7 @@
   <dimension ref="F14:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,169 +483,182 @@
       <c r="F14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="G15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="6:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="6"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="6:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="6:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="5"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="6:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>11</v>
+      <c r="G23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="7"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J17:J18"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="G21:G22"/>
@@ -653,24 +666,11 @@
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>